<commit_message>
Stworzenie wstępnej części sprawozdania
W sprawozdaniu został opisany proces porównania metod początkowych inicjalizacji wag prawdopodobieństwa oraz opisany zaostał zabieg przeprowadzenia analizy doboru najlepszych wartości parametrów.
</commit_message>
<xml_diff>
--- a/parametryzacja/1.k_set_starting_wages - wykresy.xlsx
+++ b/parametryzacja/1.k_set_starting_wages - wykresy.xlsx
@@ -1265,12 +1265,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1780,12 +1775,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>

</xml_diff>